<commit_message>
pulling in a slug; doing some hacky conditional styling - as well as showing a less-hacky way of using said slug using asset pathing
</commit_message>
<xml_diff>
--- a/google_drive_cache/1vpH2uJHUmLzJMWVV_F0aCrto4ito0vMlsTPIEXKEuS4.xlsx
+++ b/google_drive_cache/1vpH2uJHUmLzJMWVV_F0aCrto4ito0vMlsTPIEXKEuS4.xlsx
@@ -11,15 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Type</t>
+    <t>type</t>
   </si>
   <si>
-    <t>Title</t>
+    <t>title</t>
   </si>
   <si>
-    <t>Body</t>
+    <t>body</t>
+  </si>
+  <si>
+    <t>image</t>
   </si>
   <si>
     <t>Opinion</t>
@@ -38,6 +41,18 @@
   </si>
   <si>
     <t>Something something middleman</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Devsigner Conference</t>
+  </si>
+  <si>
+    <t>Speaking about Middleman @devsigner conf!</t>
+  </si>
+  <si>
+    <t>middleman_talk.png</t>
   </si>
 </sst>
 </file>
@@ -107,27 +122,44 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>